<commit_message>
implemented product class price updates from file, avoiding duplication. still need to implement the other tabs on the template
</commit_message>
<xml_diff>
--- a/app/admin/templates/pricing_update.xlsx
+++ b/app/admin/templates/pricing_update.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\admin\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E665AD-8CB3-4D09-8BFF-AE6C70A8AFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A75B7A2-3602-4E95-B0AB-8005C2C653E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27075" yWindow="1545" windowWidth="23460" windowHeight="18495" xr2:uid="{2D8CD0F5-9AAE-4DF6-8F32-0FBC2C2C8DA0}"/>
+    <workbookView xWindow="25455" yWindow="1305" windowWidth="23415" windowHeight="18495" xr2:uid="{2D8CD0F5-9AAE-4DF6-8F32-0FBC2C2C8DA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Pricing" sheetId="1" r:id="rId1"/>
     <sheet name="Customer Price Category" sheetId="2" r:id="rId2"/>
     <sheet name="Product Category Discounts" sheetId="3" r:id="rId3"/>
+    <sheet name="Product Discounts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Part Number</t>
   </si>
@@ -56,6 +57,9 @@
   </si>
   <si>
     <t>Pricing Category</t>
+  </si>
+  <si>
+    <t>Category Rank</t>
   </si>
 </sst>
 </file>
@@ -448,7 +452,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E81CF49-B215-416F-84FA-7A1F5280F76C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -498,20 +504,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEDB468-A81F-4AD9-AC6E-E372ABDBEB2A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884F3EF4-BED2-4BB2-9417-4C69A38EEDEE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>

</xml_diff>